<commit_message>
First clean version with 4 quizzes.
</commit_message>
<xml_diff>
--- a/data_raw/dicts/MGQ_dict.xlsx
+++ b/data_raw/dicts/MGQ_dict.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\projects\science\DOTS\development\packages\mpiquiz\data_raw\dicts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6638B3D4-2916-497B-AAD8-0C3C0E5CF6F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCAC2945-C425-4EFA-8053-F145B0BB1A46}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="85">
   <si>
     <t>key</t>
   </si>
@@ -88,9 +88,6 @@
     <t>&lt;h4&gt;Das Quiz ist nun beendet.&lt;/h4&gt; Bitte klicken Sie auf „Weiter", um den nächsten Test zu beginnen.</t>
   </si>
   <si>
-    <t>Sie haben {{num_correct}} aus {{num_items}} Namen richtig erkannt ({{perc_correct}}%, Punkte: {{points}}).</t>
-  </si>
-  <si>
     <t>WELCOME_METAL</t>
   </si>
   <si>
@@ -121,9 +118,6 @@
     <t>PROMPT_METAL</t>
   </si>
   <si>
-    <t>You recognized {{num_correct}} out of {{num_items}} names correctly ({{perc_correct}}%,  Points: {{points}}).</t>
-  </si>
-  <si>
     <t>THANK_YOU</t>
   </si>
   <si>
@@ -160,16 +154,127 @@
     <t>You can close the browser tab now.</t>
   </si>
   <si>
-    <t>Sie werden eine Liste mit Name sehen und sollen dort ankreuzen, welcher der Bands eine Death Metal ist. Sie haben dazu {{time_out}} Sekunden Zeit.</t>
-  </si>
-  <si>
-    <t>You will be presented with a list of names and you are asked to select all names which are Death Metal bands. You have {{time_out}} seconds to do this.</t>
-  </si>
-  <si>
-    <t>Bitte wählen Sie alle Death Metal bands aus der untenstehenden Liste aus.  Sie haben {{time_out}} Sekunden Zeit.</t>
-  </si>
-  <si>
-    <t>Please select all  Death Metal bands. You have {{time_out}} seconds.</t>
+    <t>TESTNAME_CLASSICAL</t>
+  </si>
+  <si>
+    <t>INSTRUCTIONS_CLASSICAL</t>
+  </si>
+  <si>
+    <t>PROMPT_CLASSICAL</t>
+  </si>
+  <si>
+    <t>Sie werden eine Liste mit Name sehen und sollen dort ankreuzen, welcher der Bands eine **Death Metal Band** ist. Sie haben dazu {{time_out}} Sekunden Zeit.</t>
+  </si>
+  <si>
+    <t>You will be presented with a list of names and you are asked to select all names which are **Death Metal bands**. You have {{time_out}} seconds to do this.</t>
+  </si>
+  <si>
+    <t>Bitte wählen Sie alle **Death Metal Bands** aus der untenstehenden Liste aus.  Sie haben {{time_out}} Sekunden Zeit.</t>
+  </si>
+  <si>
+    <t>Please select all  **Death Metal bands**. You have {{time_out}} seconds.</t>
+  </si>
+  <si>
+    <t>WELCOME_CLASSICAL</t>
+  </si>
+  <si>
+    <t>Classical Music  Quiz</t>
+  </si>
+  <si>
+    <t>Klassische Musik Quiz</t>
+  </si>
+  <si>
+    <t>Please select all  **violin players**. You have {{time_out}} seconds.</t>
+  </si>
+  <si>
+    <t>Willkommen zum Quiz der klassischen Musik</t>
+  </si>
+  <si>
+    <t>Welcome to the Classical Music Quiz!</t>
+  </si>
+  <si>
+    <t>Sie haben {{num_correct}} aus {{num_items}} Namen richtig erkannt ({{perc_correct}}%, Punkte: {{points}}/100).</t>
+  </si>
+  <si>
+    <t>TESTNAME_JAZZ</t>
+  </si>
+  <si>
+    <t>INSTRUCTIONS_JAZZ</t>
+  </si>
+  <si>
+    <t>PROMPT_JAZZ</t>
+  </si>
+  <si>
+    <t>WELCOME_JAZZ</t>
+  </si>
+  <si>
+    <t>Jazz Quiz</t>
+  </si>
+  <si>
+    <t>Willkommen zum Jazz Quiz</t>
+  </si>
+  <si>
+    <t>Welcome to the Jazz Quiz!</t>
+  </si>
+  <si>
+    <t>Bitte wählen Sie alle **Geiger:innen** aus der untenstehenden Liste aus.  Sie haben {{time_out}} Sekunden Zeit.</t>
+  </si>
+  <si>
+    <t>Sie werden eine Liste mit Name sehen und sollen dort ankreuzen, welche davon **Saxophonisten** sind. Sie haben dazu {{time_out}} Sekunden Zeit.</t>
+  </si>
+  <si>
+    <t>Please select all  **saxophone players**. You have {{time_out}} seconds.</t>
+  </si>
+  <si>
+    <t>Bitte wählen Sie alle Saxophonisten aus der untenstehenden Liste aus.  Sie haben {{time_out}} Sekunden Zeit.</t>
+  </si>
+  <si>
+    <t>Sie werden eine Liste mit Name sehen und sollen dort ankreuzen, welche davon **Geiger:innen** sind. Sie haben dazu {{time_out}} Sekunden Zeit.</t>
+  </si>
+  <si>
+    <t>You recognized {{num_correct}} out of {{num_items}} names correctly ({{perc_correct}}%,  Points: {{points}}/100).</t>
+  </si>
+  <si>
+    <t>TESTNAME_HIPHOP</t>
+  </si>
+  <si>
+    <t>INSTRUCTIONS_HIPHOP</t>
+  </si>
+  <si>
+    <t>PROMPT_HIPHOP</t>
+  </si>
+  <si>
+    <t>WELCOME_HIPHOP</t>
+  </si>
+  <si>
+    <t>HipHop Quiz</t>
+  </si>
+  <si>
+    <t>Sie werden eine Liste mit Name sehen und sollen dort ankreuzen, welche davon **Rapper:innen** (MCs) sind. Sie haben dazu {{time_out}} Sekunden Zeit.</t>
+  </si>
+  <si>
+    <t>Bitte wählen Sie alle **Rapper:innen/MCs** aus der untenstehenden Liste aus.  Sie haben {{time_out}} Sekunden Zeit.</t>
+  </si>
+  <si>
+    <t>Please select all  **rappers/MCs**. You have {{time_out}} seconds.</t>
+  </si>
+  <si>
+    <t>Welcome to the Hip-Hop Quiz!</t>
+  </si>
+  <si>
+    <t>Willkommen zum HipHop Quiz</t>
+  </si>
+  <si>
+    <t>Hip-Hop  Quiz</t>
+  </si>
+  <si>
+    <t>You will be presented with a list of names and you are asked to select all names which are **violin players**. You have {{time_out}} seconds to do this.</t>
+  </si>
+  <si>
+    <t>You will be presented with a list of names and you are asked to select all names which are **saxophon players**. You have {{time_out}} seconds to do this.</t>
+  </si>
+  <si>
+    <t>You will be presented with a list of names and you are asked to select all names which are **rappers** (MCs). You have {{time_out}} seconds to do this.</t>
   </si>
 </sst>
 </file>
@@ -1016,10 +1121,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C17"/>
+  <dimension ref="A1:C29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1041,7 +1146,7 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B2" t="s">
         <v>20</v>
@@ -1052,24 +1157,24 @@
     </row>
     <row r="3" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C3" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B4" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C4" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -1088,10 +1193,10 @@
         <v>12</v>
       </c>
       <c r="B6" t="s">
-        <v>22</v>
+        <v>57</v>
       </c>
       <c r="C6" t="s">
-        <v>33</v>
+        <v>70</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -1118,13 +1223,13 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
+        <v>22</v>
+      </c>
+      <c r="B9" t="s">
+        <v>26</v>
+      </c>
+      <c r="C9" t="s">
         <v>23</v>
-      </c>
-      <c r="B9" t="s">
-        <v>27</v>
-      </c>
-      <c r="C9" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -1157,62 +1262,194 @@
         <v>21</v>
       </c>
       <c r="C12" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
+        <v>27</v>
+      </c>
+      <c r="B13" t="s">
         <v>28</v>
       </c>
-      <c r="B13" t="s">
+      <c r="C13" t="s">
         <v>29</v>
-      </c>
-      <c r="C13" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
+        <v>32</v>
+      </c>
+      <c r="B14" t="s">
+        <v>33</v>
+      </c>
+      <c r="C14" t="s">
         <v>34</v>
-      </c>
-      <c r="B14" t="s">
-        <v>35</v>
-      </c>
-      <c r="C14" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
+        <v>35</v>
+      </c>
+      <c r="B15" t="s">
+        <v>36</v>
+      </c>
+      <c r="C15" t="s">
         <v>37</v>
-      </c>
-      <c r="B15" t="s">
-        <v>38</v>
-      </c>
-      <c r="C15" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
+        <v>38</v>
+      </c>
+      <c r="B16" t="s">
+        <v>39</v>
+      </c>
+      <c r="C16" t="s">
         <v>40</v>
-      </c>
-      <c r="B16" t="s">
-        <v>41</v>
-      </c>
-      <c r="C16" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
+        <v>41</v>
+      </c>
+      <c r="B17" t="s">
+        <v>42</v>
+      </c>
+      <c r="C17" t="s">
         <v>43</v>
       </c>
-      <c r="B17" t="s">
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
         <v>44</v>
       </c>
-      <c r="C17" t="s">
+      <c r="B18" t="s">
+        <v>53</v>
+      </c>
+      <c r="C18" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
         <v>45</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="C19" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>46</v>
+      </c>
+      <c r="B20" t="s">
+        <v>65</v>
+      </c>
+      <c r="C20" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>51</v>
+      </c>
+      <c r="B21" t="s">
+        <v>55</v>
+      </c>
+      <c r="C21" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>58</v>
+      </c>
+      <c r="B22" t="s">
+        <v>62</v>
+      </c>
+      <c r="C22" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>59</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C23" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>60</v>
+      </c>
+      <c r="B24" t="s">
+        <v>68</v>
+      </c>
+      <c r="C24" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>61</v>
+      </c>
+      <c r="B25" t="s">
+        <v>63</v>
+      </c>
+      <c r="C25" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>71</v>
+      </c>
+      <c r="B26" t="s">
+        <v>75</v>
+      </c>
+      <c r="C26" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>72</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="C27" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>73</v>
+      </c>
+      <c r="B28" t="s">
+        <v>77</v>
+      </c>
+      <c r="C28" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>74</v>
+      </c>
+      <c r="B29" t="s">
+        <v>80</v>
+      </c>
+      <c r="C29" t="s">
+        <v>79</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added pop singer quiz by Felix
</commit_message>
<xml_diff>
--- a/data_raw/dicts/MGQ_dict.xlsx
+++ b/data_raw/dicts/MGQ_dict.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\projects\science\DOTS\development\packages\mpiquiz\data_raw\dicts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCAC2945-C425-4EFA-8053-F145B0BB1A46}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{098FD1FF-D0F2-4CB2-A545-CC0D17A4AFD4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="96">
   <si>
     <t>key</t>
   </si>
@@ -275,6 +275,39 @@
   </si>
   <si>
     <t>You will be presented with a list of names and you are asked to select all names which are **rappers** (MCs). You have {{time_out}} seconds to do this.</t>
+  </si>
+  <si>
+    <t>TESTNAME_POP</t>
+  </si>
+  <si>
+    <t>INSTRUCTIONS_POP</t>
+  </si>
+  <si>
+    <t>PROMPT_POP</t>
+  </si>
+  <si>
+    <t>WELCOME_POP</t>
+  </si>
+  <si>
+    <t>Pop Quiz</t>
+  </si>
+  <si>
+    <t>Sie werden eine Liste mit Name sehen und sollen dort ankreuzen, welche davon **Sänger:innen**  sind. Sie haben dazu {{time_out}} Sekunden Zeit.</t>
+  </si>
+  <si>
+    <t>Bitte wählen Sie alle **Sänger:innen** aus der untenstehenden Liste aus.  Sie haben {{time_out}} Sekunden Zeit.</t>
+  </si>
+  <si>
+    <t>Willkommen zum Pop Quiz</t>
+  </si>
+  <si>
+    <t>You will be presented with a list of names and you are asked to select all names which are **singers**. You have {{time_out}} seconds to do this.</t>
+  </si>
+  <si>
+    <t>Please select all  **singers**. You have {{time_out}} seconds.</t>
+  </si>
+  <si>
+    <t>Welcome to the Pop Quiz!</t>
   </si>
 </sst>
 </file>
@@ -1121,10 +1154,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C29"/>
+  <dimension ref="A1:C33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1452,6 +1485,50 @@
         <v>79</v>
       </c>
     </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>85</v>
+      </c>
+      <c r="B30" t="s">
+        <v>89</v>
+      </c>
+      <c r="C30" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>86</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="C31" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>87</v>
+      </c>
+      <c r="B32" t="s">
+        <v>91</v>
+      </c>
+      <c r="C32" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>88</v>
+      </c>
+      <c r="B33" t="s">
+        <v>92</v>
+      </c>
+      <c r="C33" t="s">
+        <v>95</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Added result parsing function, improved scoring function, introduced equal probability for item selection
</commit_message>
<xml_diff>
--- a/data_raw/dicts/MGQ_dict.xlsx
+++ b/data_raw/dicts/MGQ_dict.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\projects\science\DOTS\development\packages\mpiquiz\data_raw\dicts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{098FD1FF-D0F2-4CB2-A545-CC0D17A4AFD4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0DB574E-1F83-4DCF-ACCB-D1CEEA9F3EA3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -193,9 +193,6 @@
     <t>Welcome to the Classical Music Quiz!</t>
   </si>
   <si>
-    <t>Sie haben {{num_correct}} aus {{num_items}} Namen richtig erkannt ({{perc_correct}}%, Punkte: {{points}}/100).</t>
-  </si>
-  <si>
     <t>TESTNAME_JAZZ</t>
   </si>
   <si>
@@ -232,9 +229,6 @@
     <t>Sie werden eine Liste mit Name sehen und sollen dort ankreuzen, welche davon **Geiger:innen** sind. Sie haben dazu {{time_out}} Sekunden Zeit.</t>
   </si>
   <si>
-    <t>You recognized {{num_correct}} out of {{num_items}} names correctly ({{perc_correct}}%,  Points: {{points}}/100).</t>
-  </si>
-  <si>
     <t>TESTNAME_HIPHOP</t>
   </si>
   <si>
@@ -308,6 +302,12 @@
   </si>
   <si>
     <t>Welcome to the Pop Quiz!</t>
+  </si>
+  <si>
+    <t>Sie haben {{num_correct}} aus {{num_items}} Namen richtig erkannt ({{perc_correct}}%,\\ {{FP}} falsch gewählt\\ und {{FN}} nicht erkannt.\\Das ergibt **{{points}}/100** Punkte.</t>
+  </si>
+  <si>
+    <t>You recognized {{num_correct}} out of {{num_items}} names correctly ({{perc_correct}}%),\\ you assigned {{FP}} wrongly,\\ and you missed {{FN}}.\\ This  yields **{{points}}/100** points.</t>
   </si>
 </sst>
 </file>
@@ -1156,8 +1156,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="C33" sqref="C33"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1226,10 +1226,10 @@
         <v>12</v>
       </c>
       <c r="B6" t="s">
-        <v>57</v>
+        <v>94</v>
       </c>
       <c r="C6" t="s">
-        <v>70</v>
+        <v>95</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -1369,10 +1369,10 @@
         <v>45</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C19" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
@@ -1380,7 +1380,7 @@
         <v>46</v>
       </c>
       <c r="B20" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C20" t="s">
         <v>54</v>
@@ -1399,134 +1399,134 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B22" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C22" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="60" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C23" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B24" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C24" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B25" t="s">
+        <v>62</v>
+      </c>
+      <c r="C25" t="s">
         <v>63</v>
-      </c>
-      <c r="C25" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B26" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C26" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="27" spans="1:3" ht="60" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C27" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B28" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C28" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B29" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C29" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B30" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C30" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="31" spans="1:3" ht="60" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C31" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B32" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C32" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B33" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C33" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Changed prompt for metal from Death metal to Black metal.
</commit_message>
<xml_diff>
--- a/data_raw/dicts/MGQ_dict.xlsx
+++ b/data_raw/dicts/MGQ_dict.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\projects\science\DOTS\development\packages\mpiquiz\data_raw\dicts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0DB574E-1F83-4DCF-ACCB-D1CEEA9F3EA3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECC6F27A-C0AC-4B72-B84C-A54FF9319C24}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -163,18 +163,6 @@
     <t>PROMPT_CLASSICAL</t>
   </si>
   <si>
-    <t>Sie werden eine Liste mit Name sehen und sollen dort ankreuzen, welcher der Bands eine **Death Metal Band** ist. Sie haben dazu {{time_out}} Sekunden Zeit.</t>
-  </si>
-  <si>
-    <t>You will be presented with a list of names and you are asked to select all names which are **Death Metal bands**. You have {{time_out}} seconds to do this.</t>
-  </si>
-  <si>
-    <t>Bitte wählen Sie alle **Death Metal Bands** aus der untenstehenden Liste aus.  Sie haben {{time_out}} Sekunden Zeit.</t>
-  </si>
-  <si>
-    <t>Please select all  **Death Metal bands**. You have {{time_out}} seconds.</t>
-  </si>
-  <si>
     <t>WELCOME_CLASSICAL</t>
   </si>
   <si>
@@ -308,6 +296,18 @@
   </si>
   <si>
     <t>You recognized {{num_correct}} out of {{num_items}} names correctly ({{perc_correct}}%),\\ you assigned {{FP}} wrongly,\\ and you missed {{FN}}.\\ This  yields **{{points}}/100** points.</t>
+  </si>
+  <si>
+    <t>Sie werden eine Liste mit Name sehen und sollen dort ankreuzen, welcher der Bands eine **BlackMetal Band** ist. Sie haben dazu {{time_out}} Sekunden Zeit.</t>
+  </si>
+  <si>
+    <t>You will be presented with a list of names and you are asked to select all names which are **BlackMetal bands**. You have {{time_out}} seconds to do this.</t>
+  </si>
+  <si>
+    <t>Bitte wählen Sie alle **Black Metal Bands** aus der untenstehenden Liste aus.  Sie haben {{time_out}} Sekunden Zeit.</t>
+  </si>
+  <si>
+    <t>Please select all  **Black Metal bands**. You have {{time_out}} seconds.</t>
   </si>
 </sst>
 </file>
@@ -1157,7 +1157,7 @@
   <dimension ref="A1:C33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1193,10 +1193,10 @@
         <v>30</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>47</v>
+        <v>92</v>
       </c>
       <c r="C3" t="s">
-        <v>48</v>
+        <v>93</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -1204,10 +1204,10 @@
         <v>31</v>
       </c>
       <c r="B4" t="s">
-        <v>49</v>
+        <v>94</v>
       </c>
       <c r="C4" t="s">
-        <v>50</v>
+        <v>95</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -1226,10 +1226,10 @@
         <v>12</v>
       </c>
       <c r="B6" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="C6" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -1358,10 +1358,10 @@
         <v>44</v>
       </c>
       <c r="B18" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="C18" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="60" x14ac:dyDescent="0.25">
@@ -1369,10 +1369,10 @@
         <v>45</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="C19" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
@@ -1380,153 +1380,153 @@
         <v>46</v>
       </c>
       <c r="B20" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="C20" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
+        <v>47</v>
+      </c>
+      <c r="B21" t="s">
         <v>51</v>
       </c>
-      <c r="B21" t="s">
-        <v>55</v>
-      </c>
       <c r="C21" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
+        <v>53</v>
+      </c>
+      <c r="B22" t="s">
         <v>57</v>
       </c>
-      <c r="B22" t="s">
-        <v>61</v>
-      </c>
       <c r="C22" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="60" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="C23" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="B24" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="C24" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="B25" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="C25" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
+        <v>65</v>
+      </c>
+      <c r="B26" t="s">
         <v>69</v>
       </c>
-      <c r="B26" t="s">
-        <v>73</v>
-      </c>
       <c r="C26" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
     </row>
     <row r="27" spans="1:3" ht="60" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
+        <v>66</v>
+      </c>
+      <c r="B27" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="B27" s="1" t="s">
-        <v>74</v>
-      </c>
       <c r="C27" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
+        <v>67</v>
+      </c>
+      <c r="B28" t="s">
         <v>71</v>
       </c>
-      <c r="B28" t="s">
-        <v>75</v>
-      </c>
       <c r="C28" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="B29" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="C29" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
+        <v>79</v>
+      </c>
+      <c r="B30" t="s">
         <v>83</v>
       </c>
-      <c r="B30" t="s">
-        <v>87</v>
-      </c>
       <c r="C30" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
     </row>
     <row r="31" spans="1:3" ht="60" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
+        <v>80</v>
+      </c>
+      <c r="B31" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="B31" s="1" t="s">
-        <v>88</v>
-      </c>
       <c r="C31" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
+        <v>81</v>
+      </c>
+      <c r="B32" t="s">
         <v>85</v>
       </c>
-      <c r="B32" t="s">
-        <v>89</v>
-      </c>
       <c r="C32" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
+        <v>82</v>
+      </c>
+      <c r="B33" t="s">
         <v>86</v>
       </c>
-      <c r="B33" t="s">
-        <v>90</v>
-      </c>
       <c r="C33" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
And yet another typo
</commit_message>
<xml_diff>
--- a/data_raw/dicts/MGQ_dict.xlsx
+++ b/data_raw/dicts/MGQ_dict.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\projects\science\DOTS\development\packages\mpiquiz\data_raw\dicts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A01B3AB-682C-4BC7-A782-F60DC618CC86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{903CF341-899E-44FF-A29F-D30F51F74208}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -328,10 +328,10 @@
     <t>You will be presented with a list of names and you are asked to select all names which are **composers of the 19th centurs** (main activity). You have {{time_out}} seconds to do this.</t>
   </si>
   <si>
-    <t>Bitte wählen Sie alle **Komponist:innen** des 19. Jhdt. (Hauptwirkungzeit) aus der untenstehenden Liste aus.  Sie haben {{time_out}} Sekunden Zeit.</t>
-  </si>
-  <si>
-    <t>Sie werden eine Liste mit Name sehen und sollen dort ankreuzen, welche davon **Komponist:innen** des 19. Jhdt. sind (Hauptwirkungzeit). Sie haben dazu {{time_out}} Sekunden Zeit.</t>
+    <t>Sie werden eine Liste mit Name sehen und sollen dort ankreuzen, welche davon **Komponisten/Komponistinnen** des 19. Jhdt. sind (Hauptwirkungzeit). Sie haben dazu {{time_out}} Sekunden Zeit.</t>
+  </si>
+  <si>
+    <t>Bitte wählen Sie alle **Komponisten/Komponistinnen** des 19. Jhdt. (Hauptwirkungzeit) aus der untenstehenden Liste aus.  Sie haben {{time_out}} Sekunden Zeit.</t>
   </si>
 </sst>
 </file>
@@ -1178,7 +1178,7 @@
   <dimension ref="A1:C37"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A35" workbookViewId="0">
-      <selection activeCell="B35" sqref="B35"/>
+      <selection activeCell="B36" sqref="B36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1562,12 +1562,12 @@
         <v>48</v>
       </c>
     </row>
-    <row r="35" spans="1:3" ht="75" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:3" ht="90" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>97</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C35" s="1" t="s">
         <v>101</v>
@@ -1578,7 +1578,7 @@
         <v>98</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="C36" s="1" t="s">
         <v>100</v>

</xml_diff>

<commit_message>
Changed metal quiz to power metal detection.
</commit_message>
<xml_diff>
--- a/data_raw/dicts/MGQ_dict.xlsx
+++ b/data_raw/dicts/MGQ_dict.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\projects\science\DOTS\development\packages\mpiquiz\data_raw\dicts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{903CF341-899E-44FF-A29F-D30F51F74208}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F992A67D-D6B4-4A51-B8D6-97B65BCC6454}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="MGQ_dict" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="181029"/>
 </workbook>
 </file>
 
@@ -298,18 +298,6 @@
     <t>You recognized {{num_correct}} out of {{num_items}} names correctly ({{perc_correct}}%),\\ you assigned {{FP}} wrongly,\\ and you missed {{FN}}.\\ This  yields **{{points}}/100** points.</t>
   </si>
   <si>
-    <t>Sie werden eine Liste mit Name sehen und sollen dort ankreuzen, welcher der Bands eine **BlackMetal Band** ist. Sie haben dazu {{time_out}} Sekunden Zeit.</t>
-  </si>
-  <si>
-    <t>You will be presented with a list of names and you are asked to select all names which are **BlackMetal bands**. You have {{time_out}} seconds to do this.</t>
-  </si>
-  <si>
-    <t>Bitte wählen Sie alle **Black Metal Bands** aus der untenstehenden Liste aus.  Sie haben {{time_out}} Sekunden Zeit.</t>
-  </si>
-  <si>
-    <t>Please select all  **Black Metal bands**. You have {{time_out}} seconds.</t>
-  </si>
-  <si>
     <t>TESTNAME_CLASSICAL_COMPOSER</t>
   </si>
   <si>
@@ -332,6 +320,18 @@
   </si>
   <si>
     <t>Bitte wählen Sie alle **Komponisten/Komponistinnen** des 19. Jhdt. (Hauptwirkungzeit) aus der untenstehenden Liste aus.  Sie haben {{time_out}} Sekunden Zeit.</t>
+  </si>
+  <si>
+    <t>Sie werden eine Liste mit Name sehen und sollen dort ankreuzen, welcher der Bands eine **Power Metal Band** ist. Sie haben dazu {{time_out}} Sekunden Zeit.</t>
+  </si>
+  <si>
+    <t>Bitte wählen Sie alle **Power Metal Bands** aus der untenstehenden Liste aus.  Sie haben {{time_out}} Sekunden Zeit.</t>
+  </si>
+  <si>
+    <t>Please select all  **Power Metal bands**. You have {{time_out}} seconds.</t>
+  </si>
+  <si>
+    <t>You will be presented with a list of names and you are asked to select all names which are **Power Metal bands**. You have {{time_out}} seconds to do this.</t>
   </si>
 </sst>
 </file>
@@ -1177,8 +1177,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A35" workbookViewId="0">
-      <selection activeCell="B36" sqref="B36"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="C35" sqref="C35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1199,400 +1199,400 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>25</v>
+        <v>10</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="90" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>30</v>
+        <v>12</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>31</v>
+        <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>94</v>
+        <v>7</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" ht="90" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>90</v>
+        <v>15</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>91</v>
+        <v>14</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>3</v>
+        <v>16</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>4</v>
+        <v>19</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>5</v>
+        <v>21</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>6</v>
+        <v>24</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>13</v>
+        <v>32</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>15</v>
+        <v>33</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>14</v>
+        <v>34</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>16</v>
+        <v>35</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>17</v>
+        <v>36</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>19</v>
+        <v>38</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>21</v>
+        <v>39</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>27</v>
+        <v>41</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>28</v>
+        <v>42</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>29</v>
+        <v>43</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>32</v>
+        <v>44</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>33</v>
+        <v>49</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="60" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>35</v>
+        <v>45</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>36</v>
+        <v>64</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>38</v>
+        <v>46</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>39</v>
+        <v>60</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>40</v>
+        <v>50</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>42</v>
+        <v>51</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>43</v>
+        <v>52</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>49</v>
+        <v>57</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>48</v>
+        <v>57</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="60" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>45</v>
+        <v>54</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>46</v>
+        <v>55</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>47</v>
+        <v>56</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>51</v>
+        <v>58</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>52</v>
+        <v>59</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>53</v>
+        <v>65</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>57</v>
+        <v>69</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>57</v>
+        <v>75</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="60" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>54</v>
+        <v>66</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>61</v>
+        <v>70</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" ht="60" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>55</v>
+        <v>67</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>63</v>
+        <v>71</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>62</v>
+        <v>72</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>56</v>
+        <v>68</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>58</v>
+        <v>74</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>59</v>
+        <v>73</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>65</v>
+        <v>79</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>69</v>
+        <v>83</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>75</v>
+        <v>83</v>
       </c>
     </row>
     <row r="27" spans="1:3" ht="60" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>66</v>
+        <v>80</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>70</v>
+        <v>84</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>67</v>
+        <v>81</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>71</v>
+        <v>85</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>72</v>
+        <v>88</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>68</v>
+        <v>82</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>74</v>
+        <v>86</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>73</v>
+        <v>89</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>79</v>
+        <v>92</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>83</v>
+        <v>49</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" ht="90" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
-        <v>80</v>
+        <v>93</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>84</v>
+        <v>98</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" ht="75" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
-        <v>81</v>
+        <v>94</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>85</v>
+        <v>99</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
-        <v>82</v>
+        <v>95</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>86</v>
+        <v>51</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>89</v>
+        <v>52</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
-        <v>96</v>
+        <v>22</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>49</v>
+        <v>26</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" ht="90" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
-        <v>97</v>
+        <v>25</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>102</v>
+        <v>20</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>101</v>
+        <v>20</v>
       </c>
     </row>
     <row r="36" spans="1:3" ht="75" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
-        <v>98</v>
+        <v>30</v>
       </c>
       <c r="B36" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="C36" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="C36" s="1" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="37" spans="1:3" ht="60" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
-        <v>99</v>
+        <v>31</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>51</v>
+        <v>101</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>52</v>
+        <v>102</v>
       </c>
     </row>
   </sheetData>

</xml_diff>